<commit_message>
submit stage 1 evidence for witval
</commit_message>
<xml_diff>
--- a/kaustubhkapatral/evidence.xlsx
+++ b/kaustubhkapatral/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -100,34 +100,58 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">7E1F865BA7A6CF671019DA83F2ADCC3869591600F027A5F92FBF8B0D9FB1F2CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">witval</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">2490F98B6DF7947FF8597CE3B81446C17B6C53B5D8AA5D7FD2C04664432619B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">witval1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BC8BD2AA1477E5ABC53C6876CD757C017F76AF0484C6F9A45E357EC25751271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">witval2</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">83C843FDBEDB635ED164B6288DD08D87BB04311BBFFDD9487350E953F35069D0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1md3e43v07r05pq54fut2kkp6ayqk8sam8usutr936sajkayp6wjq8tvzjp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C1901C379726825740EF5B0A23536BCD6C0477DE73BD8EBD8D053D36E9E4479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/8C6ABD8B8EDABCAE7D33F1C255296C4C6F4D8A9810E8BAC9FF4362FB559B4A2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3F688C1DA0B95BE4D8F7AF712702D2D05F4A26FFB48F943B072CF4519F11D41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBB7B8BEFECE5AD555EBB79F63E3FF8298BF801F2CBF55037E3072216422C331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -348,11 +372,11 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.39"/>
@@ -437,7 +461,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -452,10 +476,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -480,7 +504,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -495,10 +519,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -523,7 +547,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -538,10 +562,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +590,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -581,10 +605,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -609,7 +633,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -619,25 +643,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +686,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -672,25 +696,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +739,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -725,25 +749,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +792,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -778,25 +802,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +845,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -831,25 +855,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +898,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -884,25 +908,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -924,81 +948,81 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1047,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1033,25 +1057,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1100,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1085,12 +1109,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +1139,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1124,12 +1148,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1178,7 @@
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1163,12 +1187,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1217,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1202,12 +1226,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1226,13 +1250,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1249,15 +1273,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1279,10 +1314,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1299,35 +1334,91 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1335,12 +1426,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
   </cols>
   <sheetData>
@@ -1355,102 +1447,46 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1469,21 +1505,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1508,7 +1544,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1523,10 +1559,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1587,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1566,10 +1602,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Witval stage 3 evidence
</commit_message>
<xml_diff>
--- a/kaustubhkapatral/evidence.xlsx
+++ b/kaustubhkapatral/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <sheet name="B2" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="B5" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="B6" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="B7" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -286,10 +287,34 @@
     <t xml:space="preserve">78DF3C9D2037266F2815CE0ED414A0EFA683D7CFDC2583B56E450FC8FBD05A69</t>
   </si>
   <si>
-    <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Internal Transfer TxHash on IRISnet</t>
+    <t xml:space="preserve">519FF890B2C8A68C347B9DA7D6DF2E59D9248A04852326EED293408CCDD59547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A481851C99D767E88C30F96C61C48E0FB1FEB80A84AA029F55985CD894C3FF62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C808D28FDE0BEE6864ADF8142B75B4B3BFABCDE5A00F1F5A249E46242BFFCC8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5992C62F45ADECA548909285CF400FDDB82ACA3F75C0D05264CFE26FF279FBE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7AC8546B236E4672FABF22AE411489F2A5308E6CF194934E616E13C3BD99B82C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91B12BBCCE8ECD7CC508BA7E76643452018DCAFDC8ABA3E185453B5A19414CC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA1C1DD06721CC4C843181F1A4745B40599B180B26A856F54FE2976EFD4CC2E0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7987FA76335C203310E2D27C4C0A859B95B52FE75F962E12E4ED3082F785086A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1E85392C414980C7AE669C7AB358D03D238B47F8480991BCA667BD80D17C5835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC6A74F171548B7CDF8F3B74058BDEBABB07FFDE5A52343A3AB75D16BAEFCF94</t>
   </si>
 </sst>
 </file>
@@ -499,7 +524,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.39"/>
@@ -584,7 +609,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -627,7 +652,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -670,7 +695,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -713,7 +738,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -756,7 +781,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
   </cols>
@@ -823,7 +848,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -890,7 +915,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -957,7 +982,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1024,7 +1049,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1091,7 +1116,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1158,7 +1183,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
   </cols>
@@ -1201,7 +1226,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1280,11 +1305,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1364,10 +1389,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1379,7 +1404,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
@@ -1403,24 +1428,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1442,24 +1467,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1481,24 +1506,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1512,6 +1537,45 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1523,7 +1587,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1584,7 +1648,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1640,7 +1704,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1696,7 +1760,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
@@ -1753,7 +1817,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1811,7 +1875,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1854,7 +1918,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>

</xml_diff>